<commit_message>
iniciando a configurçao das interfaces
</commit_message>
<xml_diff>
--- a/Produtos.xlsx
+++ b/Produtos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\OneDrive\Documentos\Cartaz-Nandi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9BA0AA5C-0861-4DFC-B1BC-063C81418EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33740472-86A7-48DA-A2B7-1AB5974ADC6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{651C1E34-0767-40A5-97A8-7CA4680E2D25}"/>
   </bookViews>
@@ -427,7 +427,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>